<commit_message>
Added all necessary subflow
</commit_message>
<xml_diff>
--- a/P2-RE-Performer/Data/Config.xlsx
+++ b/P2-RE-Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f30597d3c0b08c65/Documents/UiPath/Generate-Yearly-Report/P2-RE-Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{53F025F0-0A9C-4420-97B4-56804FF4BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3B60FFD-F051-4033-94AA-0795B0A006AF}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{53F025F0-0A9C-4420-97B4-56804FF4BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAC08E79-BC83-4DD2-B195-5800B43769A0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/reports/download</t>
+  </si>
+  <si>
+    <t>in_uploadurl</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/reports/upload</t>
+  </si>
+  <si>
+    <t>in_updateurl</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/update</t>
   </si>
 </sst>
 </file>
@@ -274,6 +286,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,7 +592,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -695,8 +711,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>